<commit_message>
image upload (in the making)
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\webshop1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA93D79-9C9F-4984-AC2C-52CA57C6AF59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDF0631-6F9C-420F-9F94-E526D1589BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="6000" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Product</t>
   </si>
@@ -105,33 +105,12 @@
     <t>Nice good camera with stock Android</t>
   </si>
   <si>
-    <t>148g</t>
-  </si>
-  <si>
     <t>155g</t>
   </si>
   <si>
-    <t>166g</t>
-  </si>
-  <si>
     <t>133g</t>
   </si>
   <si>
-    <t>100g</t>
-  </si>
-  <si>
-    <t>129g</t>
-  </si>
-  <si>
-    <t>126g</t>
-  </si>
-  <si>
-    <t>120g</t>
-  </si>
-  <si>
-    <t>130g</t>
-  </si>
-  <si>
     <t>Black / Red / OceanBlue / Green</t>
   </si>
   <si>
@@ -160,6 +139,30 @@
   </si>
   <si>
     <t>Huawei</t>
+  </si>
+  <si>
+    <t>164g</t>
+  </si>
+  <si>
+    <t>113g</t>
+  </si>
+  <si>
+    <t>157g</t>
+  </si>
+  <si>
+    <t>165g</t>
+  </si>
+  <si>
+    <t>175g</t>
+  </si>
+  <si>
+    <t>192g</t>
+  </si>
+  <si>
+    <t>185g</t>
+  </si>
+  <si>
+    <t>162g</t>
   </si>
 </sst>
 </file>
@@ -483,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,13 +523,13 @@
         <v>900</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -540,13 +543,13 @@
         <v>600</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -560,13 +563,13 @@
         <v>750</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -580,13 +583,13 @@
         <v>720</v>
       </c>
       <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -600,13 +603,13 @@
         <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -620,13 +623,13 @@
         <v>240</v>
       </c>
       <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -640,13 +643,13 @@
         <v>448</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -660,13 +663,13 @@
         <v>300</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -680,13 +683,13 @@
         <v>360</v>
       </c>
       <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -700,13 +703,13 @@
         <v>600</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
         <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big update - index page, products page, products,
Index page update: Added recommended products to the page from the database.
SQL backup
Made the Product page (not done)
Added product.
Database images update.
HTML5 layout.
Styling.
Some optimisations.
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\webshop1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDF0631-6F9C-420F-9F94-E526D1589BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61012EE-9892-462B-A1C2-E9BADDC9ABB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>